<commit_message>
assignment 1 problem statement 1 completed
</commit_message>
<xml_diff>
--- a/src/test/resources/excelFiles/BookCartAutomationCases.xlsx
+++ b/src/test/resources/excelFiles/BookCartAutomationCases.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="66">
   <si>
     <t>test scenarios</t>
   </si>
@@ -209,6 +209,12 @@
   </si>
   <si>
     <t>https://bookcart.azurewebsites.net/api/ShoppingCart/12</t>
+  </si>
+  <si>
+    <t>adding 1 more book to userId 12</t>
+  </si>
+  <si>
+    <t>21</t>
   </si>
 </sst>
 </file>
@@ -299,7 +305,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -347,6 +353,9 @@
     </xf>
     <xf borderId="0" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1236,7 +1245,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="22.75"/>
+    <col customWidth="1" min="1" max="1" width="24.5"/>
     <col customWidth="1" min="2" max="2" width="47.75"/>
     <col customWidth="1" min="3" max="3" width="10.63"/>
     <col customWidth="1" min="4" max="4" width="38.63"/>
@@ -1283,12 +1292,35 @@
         <v>200.0</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="9">
+        <v>200.0</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="B2"/>
     <hyperlink r:id="rId2" ref="D2"/>
     <hyperlink r:id="rId3" ref="E2"/>
+    <hyperlink r:id="rId4" ref="B3"/>
+    <hyperlink r:id="rId5" ref="D3"/>
+    <hyperlink r:id="rId6" ref="E3"/>
   </hyperlinks>
-  <drawing r:id="rId4"/>
+  <drawing r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>